<commit_message>
Reworked Cell observations to be 1/0 and added censorship/nans (Also added basic data integrity test)
</commit_message>
<xml_diff>
--- a/lineage/data/heiser_data/Synth_data.xlsx
+++ b/lineage/data/heiser_data/Synth_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukakarginov/lineage-growth/lineage/data/heiser_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0404B3-3E5C-294C-B8DC-86B7CEC25567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821A3AE4-AB87-7843-8DFA-D9289526CB3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{522D925A-7591-9A4F-B5AC-D22920BC344D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6252B374-BF68-7345-B885-F7E11E4B37FF}">
   <dimension ref="A1:Q162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1768,7 +1768,9 @@
       <c r="Q63" s="2"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
+      <c r="A64" s="3">
+        <v>4</v>
+      </c>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>

</xml_diff>

<commit_message>
Changes to how observations are imported  (#424)
* more work

* more work

* more work
</commit_message>
<xml_diff>
--- a/lineage/data/heiser_data/Synth_data.xlsx
+++ b/lineage/data/heiser_data/Synth_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukakarginov/lineage-growth/lineage/data/heiser_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0404B3-3E5C-294C-B8DC-86B7CEC25567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821A3AE4-AB87-7843-8DFA-D9289526CB3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{522D925A-7591-9A4F-B5AC-D22920BC344D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6252B374-BF68-7345-B885-F7E11E4B37FF}">
   <dimension ref="A1:Q162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1768,7 +1768,9 @@
       <c r="Q63" s="2"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
+      <c r="A64" s="3">
+        <v>4</v>
+      </c>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>

</xml_diff>

<commit_message>
adding new [x x _] case
</commit_message>
<xml_diff>
--- a/lineage/data/heiser_data/Synth_data.xlsx
+++ b/lineage/data/heiser_data/Synth_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukakarginov/lineage-growth/lineage/data/heiser_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821A3AE4-AB87-7843-8DFA-D9289526CB3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49997F7-98F2-AC48-96D5-0EC3D0A67860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{522D925A-7591-9A4F-B5AC-D22920BC344D}"/>
   </bookViews>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6252B374-BF68-7345-B885-F7E11E4B37FF}">
   <dimension ref="A1:Q162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -971,11 +971,11 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6">
-        <v>80</v>
+        <v>145</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6">
-        <v>80</v>
+        <v>145</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>

</xml_diff>